<commit_message>
Commit 14/01/20 - 2º Falha PageObject
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A517F016-2E5F-4681-83BB-96C071FF7FF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD89F3-825A-4E0B-ABE9-7EDFF644C64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>CEP</t>
   </si>
   <si>
-    <t>Karl_Otaner2</t>
-  </si>
-  <si>
     <t>carlos.silva@rsinet.com.br</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Otaner</t>
   </si>
   <si>
-    <t>55 11 1234567</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -101,7 +95,13 @@
     <t>SAO PAULO</t>
   </si>
   <si>
-    <t>06010-060</t>
+    <t>55111234567</t>
+  </si>
+  <si>
+    <t>06010060</t>
+  </si>
+  <si>
+    <t>Karl_Otaner12</t>
   </si>
 </sst>
 </file>
@@ -145,9 +145,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,15 +464,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589AF0BB-05F7-4139-BD9B-73A9C6D4226F}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
@@ -519,41 +521,47 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Commit 15/01/20 - 1º CadastroPageObejct & Massa-OK
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD89F3-825A-4E0B-ABE9-7EDFF644C64A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23862768-1011-4813-8716-63BEAB36FF16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
     <t>06010060</t>
   </si>
   <si>
-    <t>Karl_Otaner12</t>
+    <t>Karl_Otaner30</t>
   </si>
 </sst>
 </file>
@@ -145,11 +145,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{589AF0BB-05F7-4139-BD9B-73A9C6D4226F}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,8 +561,14 @@
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L3" s="1"/>
     </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+    </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Commit 15/01/20 - 2º CadastroPageObejct & Massa - ok
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23862768-1011-4813-8716-63BEAB36FF16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FE15DA-56AB-438B-92B2-A290B3BC2880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <t>06010060</t>
   </si>
   <si>
-    <t>Karl_Otaner30</t>
+    <t>Karl_Otaner45</t>
   </si>
 </sst>
 </file>
@@ -559,6 +559,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit 15/01/20 - 3º Cadastro Positivo e Cadastro Negativo - oK
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00FE15DA-56AB-438B-92B2-A290B3BC2880}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07358064-CC07-4E93-AFB7-9FE70FB7FCA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
@@ -101,7 +101,7 @@
     <t>06010060</t>
   </si>
   <si>
-    <t>Karl_Otaner45</t>
+    <t>Karl_Otaner48</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Commit 17/01/20 - 1º Ajuste PageFactory
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07358064-CC07-4E93-AFB7-9FE70FB7FCA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A7FC0-DF2B-447D-8DEB-8EA3332AFE5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
+    <workbookView xWindow="750" yWindow="675" windowWidth="16200" windowHeight="9360" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Usuario</t>
   </si>
@@ -101,7 +103,19 @@
     <t>06010060</t>
   </si>
   <si>
-    <t>Karl_Otaner48</t>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Kensington orbit 72337 trackball with scroll ring</t>
+  </si>
+  <si>
+    <t>keyboard</t>
+  </si>
+  <si>
+    <t>Bolo</t>
+  </si>
+  <si>
+    <t>Karl_Otaner63</t>
   </si>
 </sst>
 </file>
@@ -468,7 +482,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +536,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
@@ -559,7 +573,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="4"/>
       <c r="L3" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -570,6 +584,46 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E11" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCE1C555-24A9-4E30-9A10-19DD95DC62FA}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Commit - 19/01/20 - 1° Teste de Busca por protudo da tela principal.
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A7FC0-DF2B-447D-8DEB-8EA3332AFE5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E081E47-3765-4444-8AC6-A5D5E0E5D1AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="675" windowWidth="16200" windowHeight="9360" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
     <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -115,7 +114,7 @@
     <t>Bolo</t>
   </si>
   <si>
-    <t>Karl_Otaner63</t>
+    <t>Karl_Otaner64</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Commit - 19/01/20 - 2° Implementaçao report testNG
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E081E47-3765-4444-8AC6-A5D5E0E5D1AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52808266-034D-4E6A-B6B0-3FF772A6DA16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>Bolo</t>
   </si>
   <si>
-    <t>Karl_Otaner64</t>
+    <t>Karl_Otaner77</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Commit - 21/01/20 - 1° Implem. report testNG, nos 6 cenarios, conforme ToolsQA
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52808266-034D-4E6A-B6B0-3FF772A6DA16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F0A47-3752-4248-9781-5D5B48C99826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>Bolo</t>
   </si>
   <si>
-    <t>Karl_Otaner77</t>
+    <t>Karl_Otaner93</t>
   </si>
 </sst>
 </file>
@@ -572,7 +572,7 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+      <c r="A3" s="1"/>
       <c r="L3" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Commit - 28/01/20 - Testes Ok
</commit_message>
<xml_diff>
--- a/Cadastro.xlsx
+++ b/Cadastro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos.silva\ToolsQA\TDD\TDD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204F0A47-3752-4248-9781-5D5B48C99826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD09E429-5A4F-4FC3-AA6F-3DD814B3405A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{6903E9C8-F5FB-4AEC-83FB-64855A0A6947}"/>
   </bookViews>
@@ -114,7 +114,7 @@
     <t>Bolo</t>
   </si>
   <si>
-    <t>Karl_Otaner93</t>
+    <t>Karl_Otaner135</t>
   </si>
 </sst>
 </file>

</xml_diff>